<commit_message>
Revu du Zoning et modification de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">Entrevue avec le Chef de projet pour le suivit et la cloture des sprint 1 et 2 </t>
+  </si>
+  <si>
+    <t>J'ai travaillé à la maison pour le MLD</t>
   </si>
 </sst>
 </file>
@@ -410,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,6 +468,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>43882</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finalisation du MCD, MLD et Wireframe
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>J'ai travaillé à la maison pour le MLD</t>
+  </si>
+  <si>
+    <t>J'ai revu le MCD avec M. Benzonana et M. Konutse</t>
+  </si>
+  <si>
+    <t>J'ai refait le MCD et MLD avec l'aide de M. Benzonana et j'ai pu faire un retour sur l'avancement du projet</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -131,6 +137,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -413,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +452,7 @@
       <c r="B2" s="5">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -453,7 +463,7 @@
       <c r="B3" s="6">
         <v>2.25</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -464,7 +474,7 @@
       <c r="B4" s="6">
         <v>1.5</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -475,8 +485,30 @@
       <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>43888</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>43889</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clôture du sprint 1 et du sprint 2
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>J'ai refait le MCD et MLD avec l'aide de M. Benzonana et j'ai pu faire un retour sur l'avancement du projet</t>
+  </si>
+  <si>
+    <t>Clôture du sprint 1 et 2</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,6 +514,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>43893</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Départ du sprint 3
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Clôture du sprint 1 et 2</t>
+  </si>
+  <si>
+    <t>Absence pour le recrutement</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +528,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>43894</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2.25</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Journal de travail et journal de bord
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pre-TPI\Multiplix\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Multiplix\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Absence pour le recrutement</t>
+  </si>
+  <si>
+    <t>Sprint review du sprint 2 avec le chef de projet</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,6 +542,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>43896</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
avancement sur le process d'inscription
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Sprint review du sprint 2 avec le chef de projet</t>
+  </si>
+  <si>
+    <t>Entrevue avec le chef de projet pour savoir où j'en suis et les problèmes rencontré</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +556,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>43903</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Préparation de l'environement de travail personnel
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Multiplix\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Multiplix\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766EE98-6419-4CE8-99E0-F12886B1459F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -63,12 +64,15 @@
   </si>
   <si>
     <t>Entrevue avec le chef de projet pour savoir où j'en suis et les problèmes rencontré</t>
+  </si>
+  <si>
+    <t>Préparation de l'environement de travail à la maison (sans WAMP) avec l'aide de Dorian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,11 +438,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,6 +571,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>43907</v>
+      </c>
+      <c r="B12" s="6">
+        <v>2.25</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Avancement sur la documentation et sur le mode de jeu guidé
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Multiplix\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766EE98-6419-4CE8-99E0-F12886B1459F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8672BF2D-4269-4D39-950F-ED75363D0E12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1710" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -66,7 +72,16 @@
     <t>Entrevue avec le chef de projet pour savoir où j'en suis et les problèmes rencontré</t>
   </si>
   <si>
-    <t>Préparation de l'environement de travail à la maison (sans WAMP) avec l'aide de Dorian</t>
+    <t>M. Benzonana m'a aidé à corriger les bugs qui m'empèchait d'avoir un environnement de dévelloppement fonctionnel</t>
+  </si>
+  <si>
+    <t>Préparation de l'environement de travail à la maison (sans WAMP) avec l'aide de Niclass Dorian</t>
+  </si>
+  <si>
+    <t>M. Benzonana et Meylan Benoit m'ont aidé à appliquer la fonctionnalité des calculs aléatoires</t>
+  </si>
+  <si>
+    <t>Réorganisation personnel sur le projet et avancement de la documentation</t>
   </si>
 </sst>
 </file>
@@ -439,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +594,40 @@
         <v>2.25</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>43909</v>
+      </c>
+      <c r="B13" s="6">
+        <v>5.25</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>43910</v>
+      </c>
+      <c r="B14" s="6">
+        <v>5.25</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>43914</v>
+      </c>
+      <c r="B15" s="5">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Résolution du login et du mode de jeu guidé(incomplet mais fonctionnel)
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Multiplix\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8672BF2D-4269-4D39-950F-ED75363D0E12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4245557-B43E-4835-BA50-9C258EB5D615}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1710" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Réorganisation personnel sur le projet et avancement de la documentation</t>
+  </si>
+  <si>
+    <t>Entrevue avec le chef de projet, il m'a donné du code pour que je puisse avancer</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,6 +633,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>43917</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Livrable du Pré-TPI le 03.40.2020
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord - Jungo.xlsx
+++ b/Documentation/Journal de bord - Jungo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Multiplix\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4245557-B43E-4835-BA50-9C258EB5D615}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6E686F-AAB0-45BE-B445-B61510FEAFEF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Entrevue avec le chef de projet, il m'a donné du code pour que je puisse avancer</t>
+  </si>
+  <si>
+    <t>Rendu du Pré-TPI</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +647,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>43924</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>